<commit_message>
add readingBooster. begin goin it work
</commit_message>
<xml_diff>
--- a/ExcelReaderForTableReaderLib/Концептуальная схема.xlsx
+++ b/ExcelReaderForTableReaderLib/Концептуальная схема.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="названия переменных" sheetId="1" r:id="rId1"/>
     <sheet name="Перенос фокуса" sheetId="2" r:id="rId2"/>
+    <sheet name="Думки" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="21">
   <si>
     <t>Column1</t>
   </si>
@@ -65,6 +66,24 @@
   </si>
   <si>
     <t>При переносе фокуса он не должен выходить за LastTakenRowIndex. Если TakeRows =null,   LastTakenRowIndex = int.max</t>
+  </si>
+  <si>
+    <t>MsExcelSourceReader</t>
+  </si>
+  <si>
+    <t>Предоставляет паблик интерфейс</t>
+  </si>
+  <si>
+    <t>MsExcelWorker</t>
+  </si>
+  <si>
+    <t>скрывает ньюансы работы с Excel</t>
+  </si>
+  <si>
+    <t>CellsRangeTranslator</t>
+  </si>
+  <si>
+    <t>в Excel Rnge идёт от 1, класс преобразует range в массив от 0</t>
   </si>
 </sst>
 </file>
@@ -3330,7 +3349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:AC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="AC27" sqref="AC27"/>
     </sheetView>
   </sheetViews>
@@ -4548,4 +4567,46 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>